<commit_message>
Amélioration du tableau React : couleur projections + détection NA/NS/ND
</commit_message>
<xml_diff>
--- a/Donnees/Statistiques Démographiques et sociales/Santé/Tableaux Santé de la mère et de l'enfant_Portail (1).xlsx
+++ b/Donnees/Statistiques Démographiques et sociales/Santé/Tableaux Santé de la mère et de l'enfant_Portail (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27E34ED-9F6F-4FD9-AAB2-29ADD41B6356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9780E579-8827-4287-9D61-BC82D721EA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS1" sheetId="2" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Tableau: Pourcentage de naissances vivantes ayant eu lieu au cours des 5 dernières années ayant précédé l'enquête (EDSM) accouchées par césarienne par Wilaya selon le moment de la prise de décision</t>
   </si>
   <si>
-    <t xml:space="preserve">Tableau: Pourcentage(%) de femmes de 15-49 ans qui ont reçu des soins prénatals par wilaya selon par type de prestataire de santé vu durant la grossesse  </t>
-  </si>
-  <si>
     <t>Prestataire de soins prénatals~Infirmière-sage-femme</t>
   </si>
   <si>
@@ -269,6 +266,9 @@
   </si>
   <si>
     <t>Etablissement de santé~Autre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau: Pourcentage de femmes de 15-49 ans qui ont reçu des soins prénatals par wilaya selon par type de prestataire de santé vu durant la grossesse  </t>
   </si>
 </sst>
 </file>
@@ -934,9 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -953,7 +951,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -967,28 +965,28 @@
     <row r="2" spans="1:9" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="I2" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1494,9 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1518,13 +1514,13 @@
     <row r="2" spans="1:4" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41"/>
       <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1773,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1791,7 +1787,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -1803,22 +1799,22 @@
     <row r="2" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="D2" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="E2" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>65</v>
-      </c>
       <c r="G2" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -2269,31 +2265,31 @@
     <row r="2" spans="1:10" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="G2" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="H2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="I2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="39" t="s">
-        <v>43</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2836,9 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2860,10 +2854,10 @@
     <row r="2" spans="1:4" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
@@ -3116,7 +3110,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3381,37 +3375,37 @@
     <row r="3" spans="1:12" ht="68.400000000000006" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="D3" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="F3" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="H3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="I3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="J3" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="K3" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="L3" s="44" t="s">
         <v>55</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>